<commit_message>
working copy - debug mode new logo
</commit_message>
<xml_diff>
--- a/src/test.xlsx
+++ b/src/test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="340" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -93,9 +93,6 @@
     <t>TEST2</t>
   </si>
   <si>
-    <t>TEST3</t>
-  </si>
-  <si>
     <t>LAST1</t>
   </si>
   <si>
@@ -133,6 +130,9 @@
   </si>
   <si>
     <t>ALL</t>
+  </si>
+  <si>
+    <t>TEST4</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -633,7 +633,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>21</v>
@@ -642,7 +642,7 @@
         <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I2">
         <v>1234567890</v>
@@ -651,19 +651,19 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" t="s">
         <v>35</v>
-      </c>
-      <c r="O2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -680,7 +680,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>21</v>
@@ -689,7 +689,7 @@
         <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3">
         <v>1234567890</v>
@@ -698,19 +698,19 @@
         <v>1</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
         <v>35</v>
-      </c>
-      <c r="O3" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -727,16 +727,16 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I4">
         <v>1234567890</v>
@@ -745,19 +745,19 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O4" t="s">
         <v>33</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>35</v>
-      </c>
-      <c r="O4" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>